<commit_message>
Modified names for files
</commit_message>
<xml_diff>
--- a/Web/Test_input.xlsx
+++ b/Web/Test_input.xlsx
@@ -132,10 +132,10 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -172,7 +172,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>3</v>

</xml_diff>